<commit_message>
executable jar class diagram other minor changes
</commit_message>
<xml_diff>
--- a/testdata/CogmentoTestData.xlsx
+++ b/testdata/CogmentoTestData.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shashikanth\git\automation.cogmento.com\testdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\harini\git\automation.cogmento.com\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A0B4248-8AAE-404C-BD63-AF3C91D1E0E3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Companies" sheetId="1" r:id="rId1"/>
     <sheet name="Contacts" sheetId="2" r:id="rId2"/>
     <sheet name="temp" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="104">
   <si>
     <t>Name</t>
   </si>
@@ -336,12 +337,15 @@
   </si>
   <si>
     <t>originIncUsa.exe</t>
+  </si>
+  <si>
+    <t>ABC USA Inc.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -678,11 +682,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:Z3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="X1" workbookViewId="0">
-      <selection activeCell="Z1" sqref="Z1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="22" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -854,19 +858,102 @@
         <v>102</v>
       </c>
     </row>
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="I3" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="J3" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="K3" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="L3" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="M3" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="N3" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="O3" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="P3" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="Q3" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="R3" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="S3" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="T3" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="U3" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="V3" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="W3" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="X3" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="Y3" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="Z3" s="8" t="s">
+        <v>102</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="N2" r:id="rId1"/>
-    <hyperlink ref="B2" r:id="rId2"/>
-    <hyperlink ref="O2" r:id="rId3"/>
+    <hyperlink ref="N2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B2" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="O2" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="N3" r:id="rId4" xr:uid="{7806195C-D6C9-4D32-AB80-64103E2D61F4}"/>
+    <hyperlink ref="B3" r:id="rId5" xr:uid="{D0E729C3-B2C9-428C-8950-FDDD8E6755E3}"/>
+    <hyperlink ref="O3" r:id="rId6" xr:uid="{2AA82BB1-9126-43F9-8242-5E9EB1F830A4}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId4"/>
+  <pageSetup orientation="portrait" r:id="rId7"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AK3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1130,19 +1217,19 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G2" r:id="rId1"/>
-    <hyperlink ref="K2" r:id="rId2"/>
-    <hyperlink ref="L2" r:id="rId3"/>
-    <hyperlink ref="G3" r:id="rId4"/>
-    <hyperlink ref="K3" r:id="rId5"/>
-    <hyperlink ref="L3" r:id="rId6"/>
+    <hyperlink ref="G2" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="K2" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
+    <hyperlink ref="L2" r:id="rId3" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
+    <hyperlink ref="G3" r:id="rId4" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
+    <hyperlink ref="K3" r:id="rId5" xr:uid="{00000000-0004-0000-0100-000004000000}"/>
+    <hyperlink ref="L3" r:id="rId6" xr:uid="{00000000-0004-0000-0100-000005000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1227,8 +1314,8 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="O1" r:id="rId1"/>
-    <hyperlink ref="P1" r:id="rId2"/>
+    <hyperlink ref="O1" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
+    <hyperlink ref="P1" r:id="rId2" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>